<commit_message>
JB: Completed risk assessment
</commit_message>
<xml_diff>
--- a/documentation/RiskAssessment.xlsx
+++ b/documentation/RiskAssessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\eclipse-workspace\Library_Project_BAE14\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0073F8E6-CEE9-4383-8679-24AA7C5154FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0572E698-FEF8-4F2C-89C3-81C1F7EE9EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33540" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{EDDE23BB-5AB9-488E-85F8-1BC1E343EAE3}"/>
+    <workbookView xWindow="2850" yWindow="1530" windowWidth="22665" windowHeight="11385" xr2:uid="{EDDE23BB-5AB9-488E-85F8-1BC1E343EAE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Description</t>
   </si>
@@ -56,13 +56,121 @@
   </si>
   <si>
     <t>Control Measures</t>
+  </si>
+  <si>
+    <t>Developer becomes unwell/ill</t>
+  </si>
+  <si>
+    <t>Project would be incomplete</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Developer/Divine Entity</t>
+  </si>
+  <si>
+    <t>Ask for an extension</t>
+  </si>
+  <si>
+    <t>Failure to meet the MVP</t>
+  </si>
+  <si>
+    <t>Fail the project</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Weep</t>
+  </si>
+  <si>
+    <t>Plan the project thoroughly with prioritoisation of tasks and asking for help from trainers where required</t>
+  </si>
+  <si>
+    <t>Hardware failure</t>
+  </si>
+  <si>
+    <t>Lost work and inability to complete project</t>
+  </si>
+  <si>
+    <t>Inform trainers of issues, source hardware from elsewhere</t>
+  </si>
+  <si>
+    <t>Ensure work regularly backed up to remote repo</t>
+  </si>
+  <si>
+    <t>Cannot find solution to problem</t>
+  </si>
+  <si>
+    <t>Time lost</t>
+  </si>
+  <si>
+    <t>Look through course content and notes, search for solutions online on StackOverflow</t>
+  </si>
+  <si>
+    <t>Unable to achieve sufficient test coverage</t>
+  </si>
+  <si>
+    <t>Lost marks</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Help from trainers</t>
+  </si>
+  <si>
+    <t>Attend workshop on testing, research testing and look through course content</t>
+  </si>
+  <si>
+    <t>Methods don't work as expected</t>
+  </si>
+  <si>
+    <t>Tests fail</t>
+  </si>
+  <si>
+    <t>Methods/software not working as expected</t>
+  </si>
+  <si>
+    <t>Evaluate tests and methods to determine where it is failing and correct as required</t>
+  </si>
+  <si>
+    <t>Write method and test code carefully. Could implement test-driven development or test methods as created</t>
+  </si>
+  <si>
+    <t>Project would not function as required</t>
+  </si>
+  <si>
+    <t>Correct method and code</t>
+  </si>
+  <si>
+    <t>Test methods, check methods working as expected as methods created</t>
+  </si>
+  <si>
+    <t>Incorrect user input</t>
+  </si>
+  <si>
+    <t>API stop working due to exceptions</t>
+  </si>
+  <si>
+    <t>Refactor methods to throw exceptions</t>
+  </si>
+  <si>
+    <t>Develop code to expect exceptions as the project is built</t>
+  </si>
+  <si>
+    <t>Hand hygeine and avoid extreme sports</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,19 +178,59 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -91,8 +239,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,45 +567,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6F0D71-9FCB-499E-89DE-D2508B0A46C7}">
-  <dimension ref="B3:H3"/>
+  <dimension ref="B3:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
JB: Added risk matrix
</commit_message>
<xml_diff>
--- a/documentation/RiskAssessment.xlsx
+++ b/documentation/RiskAssessment.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\eclipse-workspace\Library_Project_BAE14\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0572E698-FEF8-4F2C-89C3-81C1F7EE9EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0709C815-1B4B-4069-AD8F-40A7430330D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="1530" windowWidth="22665" windowHeight="11385" xr2:uid="{EDDE23BB-5AB9-488E-85F8-1BC1E343EAE3}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{EDDE23BB-5AB9-488E-85F8-1BC1E343EAE3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Risk Assessment" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -570,7 +571,7 @@
   <dimension ref="B3:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +711,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>15</v>
@@ -894,4 +895,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F8C7B1-4724-4054-8A0B-31074674FC17}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>